<commit_message>
add schematics and PCB files
</commit_message>
<xml_diff>
--- a/EHD/weight-model.xlsx
+++ b/EHD/weight-model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickos01/Desktop/MolecularKinetics/EHD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88F9D6E-5050-5D4A-BF6C-EB91832E8F00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DEBAE1-9DF9-1342-8988-8CF51C9E3DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="27240" windowHeight="16860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="500" windowWidth="27240" windowHeight="16860" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thrust and Weight" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="328">
   <si>
     <t>Coil form</t>
   </si>
@@ -978,12 +978,6 @@
     <t>pf capacitance</t>
   </si>
   <si>
-    <t>1050/46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2*420/46 </t>
-  </si>
-  <si>
     <t>66/46</t>
   </si>
   <si>
@@ -996,9 +990,6 @@
     <t>Toroids</t>
   </si>
   <si>
-    <t>Measurements on actual sizes</t>
-  </si>
-  <si>
     <t>Ae cm^2</t>
   </si>
   <si>
@@ -1021,6 +1012,12 @@
   </si>
   <si>
     <t>battery 4X 16350</t>
+  </si>
+  <si>
+    <t>Measurements of actual sizes</t>
+  </si>
+  <si>
+    <t>(60/46) 80</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1031,7 @@
     <numFmt numFmtId="167" formatCode="0.0E+00"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1123,16 +1120,8 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1148,6 +1137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1289,7 +1284,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1360,8 +1355,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5018,8 +5016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Y119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5211,7 +5209,7 @@
         <v>165</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>166</v>
@@ -5675,6 +5673,9 @@
       <c r="K16" s="7">
         <v>121.5</v>
       </c>
+      <c r="L16" t="s">
+        <v>327</v>
+      </c>
       <c r="M16" s="2">
         <f>PI()*(M10/2)^2</f>
         <v>0.63617251235193317</v>
@@ -5718,7 +5719,7 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="48" t="s">
         <v>61</v>
       </c>
       <c r="M17" s="4">
@@ -5983,7 +5984,7 @@
         <v>165</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.2">
@@ -6303,7 +6304,7 @@
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G57" s="2">
         <f>B57</f>
@@ -7307,8 +7308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AG125"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M117" sqref="M117"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7330,34 +7331,34 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>11.1</v>
+        <v>10</v>
       </c>
       <c r="C3">
+        <v>13.3</v>
+      </c>
+      <c r="D3" s="49">
+        <v>13.3</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>13.3</v>
+      </c>
+      <c r="H3" s="49">
+        <v>13.3</v>
+      </c>
+      <c r="I3">
+        <v>13.3</v>
+      </c>
+      <c r="J3" s="49">
         <v>14.8</v>
       </c>
-      <c r="D3">
-        <v>14.8</v>
-      </c>
-      <c r="E3">
-        <v>11.1</v>
-      </c>
-      <c r="F3">
-        <v>11.1</v>
-      </c>
-      <c r="G3">
-        <v>14.8</v>
-      </c>
-      <c r="H3">
-        <v>14.8</v>
-      </c>
-      <c r="I3">
-        <v>14.8</v>
-      </c>
-      <c r="J3">
-        <v>14.8</v>
-      </c>
       <c r="K3">
-        <v>14.8</v>
+        <v>13.3</v>
       </c>
       <c r="L3" t="s">
         <v>100</v>
@@ -7367,7 +7368,7 @@
       </c>
       <c r="N3">
         <f>B3*2</f>
-        <v>22.2</v>
+        <v>20</v>
       </c>
       <c r="O3" t="s">
         <v>134</v>
@@ -7383,7 +7384,7 @@
       <c r="C4">
         <v>0.49</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="49">
         <v>0.49</v>
       </c>
       <c r="E4">
@@ -7395,13 +7396,13 @@
       <c r="G4">
         <v>0.626</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="49">
         <v>0.626</v>
       </c>
       <c r="I4">
         <v>0.626</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="49">
         <v>0.626</v>
       </c>
       <c r="K4">
@@ -7415,13 +7416,13 @@
       </c>
       <c r="N4">
         <f>K3*2</f>
-        <v>29.6</v>
+        <v>26.6</v>
       </c>
       <c r="O4" t="s">
         <v>134</v>
       </c>
       <c r="P4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -7431,7 +7432,7 @@
       <c r="C5">
         <v>625000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="49">
         <v>625000</v>
       </c>
       <c r="E5">
@@ -7443,13 +7444,13 @@
       <c r="G5">
         <v>625000</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="49">
         <v>625000</v>
       </c>
       <c r="I5">
         <v>625000</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="49">
         <v>625000</v>
       </c>
       <c r="K5">
@@ -7469,7 +7470,7 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="49">
         <v>4</v>
       </c>
       <c r="E6">
@@ -7481,13 +7482,13 @@
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="49">
         <v>3</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="49">
         <v>3</v>
       </c>
       <c r="K6">
@@ -7510,7 +7511,7 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="49">
         <v>4</v>
       </c>
       <c r="E7">
@@ -7522,13 +7523,13 @@
       <c r="G7">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="49">
         <v>4</v>
       </c>
       <c r="I7">
         <v>4</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="49">
         <v>4</v>
       </c>
       <c r="K7">
@@ -7544,43 +7545,43 @@
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <f t="shared" ref="B8:K8" si="0">(B3*10^8)/(B4*B5*B6*B7)</f>
-        <v>302.0408163265306</v>
+        <v>272.10884353741494</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
-        <v>302.0408163265306</v>
-      </c>
-      <c r="D8" s="5">
+        <v>271.42857142857144</v>
+      </c>
+      <c r="D8" s="50">
         <f t="shared" si="0"/>
-        <v>302.0408163265306</v>
+        <v>271.42857142857144</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>236.42172523961662</v>
+        <v>212.99254526091588</v>
       </c>
       <c r="F8" s="5">
         <f>(F3*10^8)/(F4*F5*F6*F7)</f>
-        <v>236.42172523961662</v>
+        <v>212.99254526091588</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
-        <v>315.22896698615551</v>
-      </c>
-      <c r="H8" s="5">
+        <v>283.28008519701808</v>
+      </c>
+      <c r="H8" s="50">
         <f t="shared" si="0"/>
-        <v>315.22896698615551</v>
+        <v>283.28008519701808</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="0"/>
-        <v>315.22896698615551</v>
-      </c>
-      <c r="J8" s="5">
+        <v>283.28008519701808</v>
+      </c>
+      <c r="J8" s="50">
         <f>(J3*10^8)/(J4*J5*J6*J7)</f>
         <v>315.22896698615551</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="0"/>
-        <v>236.42172523961662</v>
+        <v>212.46006389776358</v>
       </c>
       <c r="L8" t="s">
         <v>99</v>
@@ -7592,43 +7593,43 @@
     <row r="9" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <f t="shared" ref="B9:K9" si="1">B8/10</f>
-        <v>30.204081632653061</v>
+        <v>27.210884353741495</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="1"/>
-        <v>30.204081632653061</v>
-      </c>
-      <c r="D9" s="4">
+        <v>27.142857142857146</v>
+      </c>
+      <c r="D9" s="51">
         <f t="shared" si="1"/>
-        <v>30.204081632653061</v>
+        <v>27.142857142857146</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>23.642172523961662</v>
+        <v>21.299254526091588</v>
       </c>
       <c r="F9" s="4">
         <f>F8/10</f>
-        <v>23.642172523961662</v>
+        <v>21.299254526091588</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="1"/>
-        <v>31.522896698615551</v>
-      </c>
-      <c r="H9" s="4">
+        <v>28.328008519701807</v>
+      </c>
+      <c r="H9" s="51">
         <f t="shared" si="1"/>
-        <v>31.522896698615551</v>
+        <v>28.328008519701807</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="1"/>
-        <v>31.522896698615551</v>
-      </c>
-      <c r="J9" s="4">
+        <v>28.328008519701807</v>
+      </c>
+      <c r="J9" s="51">
         <f>J8/10</f>
         <v>31.522896698615551</v>
       </c>
       <c r="K9" s="4">
         <f t="shared" si="1"/>
-        <v>23.642172523961662</v>
+        <v>21.246006389776358</v>
       </c>
       <c r="L9" t="s">
         <v>99</v>
@@ -7641,6 +7642,9 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="J10" s="49"/>
       <c r="N10" s="37" t="s">
         <v>283</v>
       </c>
@@ -7661,7 +7665,7 @@
       <c r="C11" s="7">
         <v>160</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="49">
         <v>250</v>
       </c>
       <c r="E11" s="7">
@@ -7673,13 +7677,13 @@
       <c r="G11" s="7">
         <v>100</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="49">
         <v>130</v>
       </c>
       <c r="I11" s="7">
         <v>160</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="49">
         <v>160</v>
       </c>
       <c r="K11" s="7">
@@ -7711,43 +7715,43 @@
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <f>B11/B3</f>
-        <v>9.0090090090090094</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2">
         <f>C11/C3</f>
-        <v>10.810810810810811</v>
-      </c>
-      <c r="D12" s="2">
+        <v>12.030075187969924</v>
+      </c>
+      <c r="D12" s="52">
         <f>D11/D3</f>
-        <v>16.891891891891891</v>
+        <v>18.796992481203006</v>
       </c>
       <c r="E12" s="2">
         <f>E11/E3</f>
-        <v>9.0090090090090094</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2">
         <f>F11/F3</f>
-        <v>11.711711711711713</v>
+        <v>13</v>
       </c>
       <c r="G12" s="2">
         <f>G11/G3</f>
-        <v>6.7567567567567561</v>
-      </c>
-      <c r="H12" s="2">
+        <v>7.518796992481203</v>
+      </c>
+      <c r="H12" s="52">
         <f>H11/H3</f>
-        <v>8.7837837837837842</v>
+        <v>9.7744360902255636</v>
       </c>
       <c r="I12" s="2">
         <f>I11/I3</f>
-        <v>10.810810810810811</v>
-      </c>
-      <c r="J12" s="2">
+        <v>12.030075187969924</v>
+      </c>
+      <c r="J12" s="52">
         <f>J11/J3</f>
         <v>10.810810810810811</v>
       </c>
       <c r="K12" s="2">
         <f>K11/K3</f>
-        <v>10.810810810810811</v>
+        <v>12.030075187969924</v>
       </c>
       <c r="L12" t="s">
         <v>122</v>
@@ -7757,11 +7761,11 @@
       </c>
       <c r="O12" s="36">
         <f>B12/2</f>
-        <v>4.5045045045045047</v>
+        <v>5</v>
       </c>
       <c r="P12" s="43">
         <f>H12/2</f>
-        <v>4.3918918918918921</v>
+        <v>4.8872180451127818</v>
       </c>
       <c r="Q12" s="36"/>
       <c r="R12" t="s">
@@ -7801,43 +7805,43 @@
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <f>B12/2</f>
-        <v>4.5045045045045047</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
         <f>C12/2</f>
-        <v>5.4054054054054053</v>
-      </c>
-      <c r="D13" s="2">
+        <v>6.0150375939849621</v>
+      </c>
+      <c r="D13" s="52">
         <f>D12/2</f>
-        <v>8.4459459459459456</v>
+        <v>9.3984962406015029</v>
       </c>
       <c r="E13" s="2">
         <f>E12/2</f>
-        <v>4.5045045045045047</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2">
         <f>F12/2</f>
-        <v>5.8558558558558564</v>
+        <v>6.5</v>
       </c>
       <c r="G13" s="2">
         <f>G12/2</f>
-        <v>3.3783783783783781</v>
-      </c>
-      <c r="H13" s="2">
+        <v>3.7593984962406015</v>
+      </c>
+      <c r="H13" s="52">
         <f>H12/2</f>
-        <v>4.3918918918918921</v>
+        <v>4.8872180451127818</v>
       </c>
       <c r="I13" s="2">
         <f>I12/2</f>
-        <v>5.4054054054054053</v>
-      </c>
-      <c r="J13" s="2">
+        <v>6.0150375939849621</v>
+      </c>
+      <c r="J13" s="52">
         <f>J12/2</f>
         <v>5.4054054054054053</v>
       </c>
       <c r="K13" s="2">
         <f>K12/2</f>
-        <v>5.4054054054054053</v>
+        <v>6.0150375939849621</v>
       </c>
       <c r="L13" t="s">
         <v>124</v>
@@ -7847,11 +7851,11 @@
       </c>
       <c r="O13" s="36">
         <f>O12*O11</f>
-        <v>0.15765765765765768</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="P13" s="43">
         <f>P12*P11</f>
-        <v>0.15371621621621623</v>
+        <v>0.17105263157894737</v>
       </c>
       <c r="Q13" s="36"/>
       <c r="R13">
@@ -7903,16 +7907,19 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="J14" s="49"/>
       <c r="N14" s="42" t="s">
         <v>121</v>
       </c>
       <c r="O14" s="36">
         <f>O12^2 * O11</f>
-        <v>0.71016962908854819</v>
+        <v>0.87500000000000011</v>
       </c>
       <c r="P14" s="43">
         <f>P12^2 * P11</f>
-        <v>0.67510500365230108</v>
+        <v>0.83597150771666018</v>
       </c>
       <c r="Q14" s="36"/>
       <c r="R14">
@@ -7970,8 +7977,8 @@
       <c r="C15" s="7">
         <v>300</v>
       </c>
-      <c r="D15" s="7">
-        <v>300</v>
+      <c r="D15" s="49">
+        <v>333</v>
       </c>
       <c r="E15" s="7">
         <v>300</v>
@@ -7982,13 +7989,13 @@
       <c r="G15" s="7">
         <v>300</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="49">
         <v>300</v>
       </c>
       <c r="I15" s="7">
         <v>300</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="49">
         <v>300</v>
       </c>
       <c r="K15" s="7">
@@ -8002,11 +8009,11 @@
       </c>
       <c r="O15" s="36">
         <f>2*O14</f>
-        <v>1.4203392581770964</v>
+        <v>1.7500000000000002</v>
       </c>
       <c r="P15" s="43">
         <f>2*P14</f>
-        <v>1.3502100073046022</v>
+        <v>1.6719430154333204</v>
       </c>
       <c r="Q15" s="36"/>
       <c r="R15">
@@ -8060,46 +8067,46 @@
     <row r="16" spans="1:33" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <f>B15/B3*B6</f>
-        <v>81.081081081081081</v>
+        <v>90</v>
       </c>
       <c r="C16" s="5">
         <f>C15/C3*C6</f>
-        <v>81.081081081081081</v>
-      </c>
-      <c r="D16" s="5">
+        <v>90.225563909774436</v>
+      </c>
+      <c r="D16" s="50">
         <f>D15/D3*D6</f>
-        <v>81.081081081081081</v>
+        <v>100.15037593984962</v>
       </c>
       <c r="E16" s="5">
         <f>E15/E3*E6</f>
-        <v>81.081081081081081</v>
+        <v>90</v>
       </c>
       <c r="F16" s="5">
         <f>F15/F3*F6</f>
-        <v>81.081081081081081</v>
+        <v>90</v>
       </c>
       <c r="G16" s="5">
         <f>G15/G3*G6</f>
-        <v>60.810810810810807</v>
-      </c>
-      <c r="H16" s="5">
+        <v>67.669172932330824</v>
+      </c>
+      <c r="H16" s="50">
         <f>H15/H3*H6</f>
-        <v>60.810810810810807</v>
+        <v>67.669172932330824</v>
       </c>
       <c r="I16" s="5">
         <f>I15/I3*I6</f>
-        <v>60.810810810810807</v>
-      </c>
-      <c r="J16" s="5">
+        <v>67.669172932330824</v>
+      </c>
+      <c r="J16" s="50">
         <f>J15/J3*J6</f>
         <v>60.810810810810807</v>
       </c>
       <c r="K16" s="5">
         <f>K15/K3*K6</f>
-        <v>81.081081081081081</v>
+        <v>90.225563909774436</v>
       </c>
       <c r="L16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N16" s="44"/>
       <c r="O16" s="45"/>
@@ -8162,9 +8169,9 @@
         <f>C11/C15</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="52">
         <f>D11/D15</f>
-        <v>0.83333333333333337</v>
+        <v>0.75075075075075071</v>
       </c>
       <c r="E17" s="2">
         <f>E11/E15</f>
@@ -8178,7 +8185,7 @@
         <f>G11/G15</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="52">
         <f>H11/H15</f>
         <v>0.43333333333333335</v>
       </c>
@@ -8186,7 +8193,7 @@
         <f>I11/I15</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="52">
         <f>J11/J15</f>
         <v>0.53333333333333333</v>
       </c>
@@ -8217,6 +8224,9 @@
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="J18" s="49"/>
       <c r="T18">
         <v>330</v>
       </c>
@@ -8238,34 +8248,34 @@
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B19" s="7">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="C19" s="7">
-        <v>267</v>
-      </c>
-      <c r="D19" s="7">
-        <v>267</v>
+        <v>300</v>
+      </c>
+      <c r="D19" s="49">
+        <v>300</v>
       </c>
       <c r="E19" s="7">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="F19" s="7">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="G19" s="7">
-        <v>267</v>
-      </c>
-      <c r="H19" s="7">
-        <v>267</v>
+        <v>300</v>
+      </c>
+      <c r="H19" s="49">
+        <v>300</v>
       </c>
       <c r="I19" s="7">
-        <v>267</v>
-      </c>
-      <c r="J19" s="7">
-        <v>267</v>
+        <v>300</v>
+      </c>
+      <c r="J19" s="49">
+        <v>300</v>
       </c>
       <c r="K19" s="7">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="L19" t="s">
         <v>305</v>
@@ -8290,6 +8300,9 @@
       </c>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="J20" s="49"/>
       <c r="R20" s="31"/>
       <c r="T20">
         <v>660</v>
@@ -8313,43 +8326,43 @@
     <row r="21" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B21">
         <f>B15*B19</f>
-        <v>80100</v>
+        <v>90000</v>
       </c>
       <c r="C21">
         <f>C15*C19</f>
-        <v>80100</v>
-      </c>
-      <c r="D21">
+        <v>90000</v>
+      </c>
+      <c r="D21" s="49">
         <f>D15*D19</f>
-        <v>80100</v>
+        <v>99900</v>
       </c>
       <c r="E21">
         <f>E15*E19</f>
-        <v>80100</v>
+        <v>90000</v>
       </c>
       <c r="F21">
         <f>F15*F19</f>
-        <v>80100</v>
+        <v>90000</v>
       </c>
       <c r="G21">
         <f>G15*G19</f>
-        <v>80100</v>
-      </c>
-      <c r="H21">
+        <v>90000</v>
+      </c>
+      <c r="H21" s="49">
         <f>H15*H19</f>
-        <v>80100</v>
+        <v>90000</v>
       </c>
       <c r="I21">
         <f>I15*I19</f>
-        <v>80100</v>
-      </c>
-      <c r="J21">
+        <v>90000</v>
+      </c>
+      <c r="J21" s="49">
         <f>J15*J19</f>
-        <v>80100</v>
+        <v>90000</v>
       </c>
       <c r="K21">
         <f>K15*K19</f>
-        <v>80100</v>
+        <v>90000</v>
       </c>
       <c r="L21" t="s">
         <v>126</v>
@@ -8361,43 +8374,43 @@
     <row r="22" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <f>B11/B21*1000</f>
-        <v>1.2484394506866416</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" ref="C22:K22" si="4">C11/C21*1000</f>
-        <v>1.9975031210986267</v>
-      </c>
-      <c r="D22" s="2">
+        <v>1.7777777777777779</v>
+      </c>
+      <c r="D22" s="52">
         <f t="shared" si="4"/>
-        <v>3.1210986267166039</v>
+        <v>2.5025025025025025</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="4"/>
-        <v>1.2484394506866416</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="4"/>
-        <v>1.6229712858926342</v>
+        <v>1.4444444444444444</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="4"/>
-        <v>1.2484394506866416</v>
-      </c>
-      <c r="H22" s="2">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="H22" s="52">
         <f t="shared" si="4"/>
-        <v>1.6229712858926342</v>
+        <v>1.4444444444444444</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="4"/>
-        <v>1.9975031210986267</v>
-      </c>
-      <c r="J22" s="2">
+        <v>1.7777777777777779</v>
+      </c>
+      <c r="J22" s="52">
         <f t="shared" si="4"/>
-        <v>1.9975031210986267</v>
+        <v>1.7777777777777779</v>
       </c>
       <c r="K22" s="2">
         <f t="shared" si="4"/>
-        <v>1.9975031210986267</v>
+        <v>1.7777777777777779</v>
       </c>
       <c r="L22" t="s">
         <v>130</v>
@@ -8407,13 +8420,16 @@
       </c>
       <c r="R22" s="31"/>
       <c r="T22" s="17" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="AA22" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="J23" s="49"/>
       <c r="T23">
         <v>40</v>
       </c>
@@ -8437,7 +8453,7 @@
       <c r="C24">
         <v>300</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="49">
         <v>300</v>
       </c>
       <c r="E24">
@@ -8449,13 +8465,13 @@
       <c r="G24">
         <v>300</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="49">
         <v>300</v>
       </c>
       <c r="I24">
         <v>300</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="49">
         <v>300</v>
       </c>
       <c r="K24">
@@ -8488,7 +8504,7 @@
       <c r="C25">
         <v>300</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="49">
         <v>300</v>
       </c>
       <c r="E25">
@@ -8500,13 +8516,13 @@
       <c r="G25">
         <v>300</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="49">
         <v>300</v>
       </c>
       <c r="I25">
         <v>300</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="49">
         <v>300</v>
       </c>
       <c r="K25">
@@ -8537,43 +8553,43 @@
     <row r="26" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B26" s="4">
         <f>B24*B13</f>
-        <v>1351.3513513513515</v>
+        <v>1500</v>
       </c>
       <c r="C26" s="4">
         <f>C24*C13</f>
-        <v>1621.6216216216217</v>
-      </c>
-      <c r="D26" s="4">
+        <v>1804.5112781954886</v>
+      </c>
+      <c r="D26" s="51">
         <f>D24*D13</f>
-        <v>2533.7837837837837</v>
+        <v>2819.5488721804509</v>
       </c>
       <c r="E26" s="4">
         <f>E24*E13</f>
-        <v>1351.3513513513515</v>
+        <v>1500</v>
       </c>
       <c r="F26" s="4">
         <f>F24*F13</f>
-        <v>1756.7567567567569</v>
+        <v>1950</v>
       </c>
       <c r="G26" s="4">
         <f>G24*G13</f>
-        <v>1013.5135135135134</v>
-      </c>
-      <c r="H26" s="4">
+        <v>1127.8195488721803</v>
+      </c>
+      <c r="H26" s="51">
         <f>H24*H13</f>
-        <v>1317.5675675675677</v>
+        <v>1466.1654135338345</v>
       </c>
       <c r="I26" s="4">
         <f>I24*I13</f>
-        <v>1621.6216216216217</v>
-      </c>
-      <c r="J26" s="4">
+        <v>1804.5112781954886</v>
+      </c>
+      <c r="J26" s="51">
         <f>J24*J13</f>
         <v>1621.6216216216217</v>
       </c>
       <c r="K26" s="4">
         <f>K24*K13</f>
-        <v>1621.6216216216217</v>
+        <v>1804.5112781954886</v>
       </c>
       <c r="L26" t="s">
         <v>127</v>
@@ -8598,7 +8614,7 @@
         <v>1</v>
       </c>
       <c r="AD26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.2">
@@ -8610,9 +8626,9 @@
         <f>C25*C17</f>
         <v>160</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="49">
         <f>D25*D17</f>
-        <v>250</v>
+        <v>225.22522522522522</v>
       </c>
       <c r="E27">
         <f>E25*E17</f>
@@ -8626,7 +8642,7 @@
         <f>G25*G17</f>
         <v>100</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="49">
         <f>H25*H17</f>
         <v>130</v>
       </c>
@@ -8634,7 +8650,7 @@
         <f>I25*I17</f>
         <v>160</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="49">
         <f>J24*J17</f>
         <v>160</v>
       </c>
@@ -8649,65 +8665,65 @@
         <v>280</v>
       </c>
       <c r="T27">
-        <v>270</v>
-      </c>
-      <c r="U27" s="48">
-        <v>3.9E-2</v>
+        <v>420</v>
+      </c>
+      <c r="U27">
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <f>B24*(B22/1000)</f>
-        <v>0.37453183520599254</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" ref="C28:K28" si="5">C24*(C22/1000)</f>
-        <v>0.59925093632958804</v>
-      </c>
-      <c r="D28" s="2">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="D28" s="52">
         <f t="shared" si="5"/>
-        <v>0.93632958801498123</v>
+        <v>0.75075075075075071</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="5"/>
-        <v>0.37453183520599254</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="5"/>
-        <v>0.48689138576779023</v>
+        <v>0.43333333333333329</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="5"/>
-        <v>0.37453183520599254</v>
-      </c>
-      <c r="H28" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H28" s="52">
         <f t="shared" si="5"/>
-        <v>0.48689138576779023</v>
+        <v>0.43333333333333329</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="5"/>
-        <v>0.59925093632958804</v>
-      </c>
-      <c r="J28" s="2">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="J28" s="52">
         <f t="shared" si="5"/>
-        <v>0.59925093632958804</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" si="5"/>
-        <v>0.59925093632958804</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="L28" t="s">
         <v>129</v>
       </c>
       <c r="R28" s="31"/>
       <c r="T28">
-        <v>330</v>
-      </c>
-      <c r="U28" s="48">
-        <v>4.2000000000000003E-2</v>
+        <v>660</v>
+      </c>
+      <c r="U28">
+        <v>6.2E-2</v>
       </c>
       <c r="AA28" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="AB28">
         <v>3.2000000000000001E-2</v>
@@ -8720,11 +8736,14 @@
       </c>
     </row>
     <row r="29" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="J29" s="49"/>
       <c r="T29">
-        <v>420</v>
+        <v>1162</v>
       </c>
       <c r="U29">
-        <v>4.8000000000000001E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="AA29" t="s">
         <v>152</v>
@@ -8750,7 +8769,7 @@
         <f t="shared" si="6"/>
         <v>2.4696969696969697</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="51">
         <f t="shared" si="6"/>
         <v>2.4696969696969697</v>
       </c>
@@ -8766,7 +8785,7 @@
         <f t="shared" si="6"/>
         <v>2.4696969696969697</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="51">
         <f t="shared" si="6"/>
         <v>2.4696969696969697</v>
       </c>
@@ -8774,7 +8793,7 @@
         <f t="shared" si="6"/>
         <v>2.4696969696969697</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="51">
         <f t="shared" si="6"/>
         <v>2.4696969696969697</v>
       </c>
@@ -8787,10 +8806,10 @@
       </c>
       <c r="R30" s="31"/>
       <c r="T30">
-        <v>660</v>
+        <v>3000</v>
       </c>
       <c r="U30">
-        <v>6.2E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AA30" t="s">
         <v>84</v>
@@ -8803,14 +8822,11 @@
       </c>
     </row>
     <row r="31" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="T31">
-        <v>1162</v>
-      </c>
-      <c r="U31">
-        <v>8.2000000000000003E-2</v>
-      </c>
+      <c r="D31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="J31" s="49"/>
       <c r="AA31" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AB31">
         <f>(AB24-AB23)/2*AB25/100</f>
@@ -8827,52 +8843,46 @@
     <row r="32" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B32" s="5">
         <f t="shared" ref="B32:K32" si="7">B26/B30</f>
-        <v>547.17293981097669</v>
+        <v>607.36196319018404</v>
       </c>
       <c r="C32" s="5">
         <f t="shared" si="7"/>
-        <v>656.60752777317191</v>
-      </c>
-      <c r="D32" s="5">
+        <v>730.66100834909355</v>
+      </c>
+      <c r="D32" s="50">
         <f t="shared" ref="D32" si="8">D26/D30</f>
-        <v>1025.9492621455811</v>
+        <v>1141.6578255454585</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" si="7"/>
-        <v>547.17293981097669</v>
+        <v>607.36196319018404</v>
       </c>
       <c r="F32" s="5">
         <f>F26/F30</f>
-        <v>711.32482175426969</v>
+        <v>789.57055214723925</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" ref="G32" si="9">G26/G30</f>
-        <v>410.3797048582324</v>
-      </c>
-      <c r="H32" s="5">
+        <v>456.66313021818343</v>
+      </c>
+      <c r="H32" s="50">
         <f t="shared" si="7"/>
-        <v>533.4936163157023</v>
+        <v>593.66206928363852</v>
       </c>
       <c r="I32" s="5">
         <f t="shared" si="7"/>
-        <v>656.60752777317191</v>
-      </c>
-      <c r="J32" s="5">
+        <v>730.66100834909355</v>
+      </c>
+      <c r="J32" s="50">
         <f>J26/J30</f>
         <v>656.60752777317191</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="7"/>
-        <v>656.60752777317191</v>
+        <v>730.66100834909355</v>
       </c>
       <c r="L32" t="s">
         <v>132</v>
-      </c>
-      <c r="T32">
-        <v>3000</v>
-      </c>
-      <c r="U32">
-        <v>0.14000000000000001</v>
       </c>
       <c r="AA32" t="s">
         <v>268</v>
@@ -8898,9 +8908,9 @@
         <f t="shared" si="10"/>
         <v>64.785276073619627</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="50">
         <f t="shared" ref="D33" si="11">D27/D30</f>
-        <v>101.22699386503068</v>
+        <v>91.195489968496105</v>
       </c>
       <c r="E33" s="5">
         <f t="shared" si="10"/>
@@ -8914,7 +8924,7 @@
         <f t="shared" ref="G33" si="12">G27/G30</f>
         <v>40.490797546012267</v>
       </c>
-      <c r="H33" s="5">
+      <c r="H33" s="50">
         <f t="shared" si="10"/>
         <v>52.638036809815951</v>
       </c>
@@ -8922,7 +8932,7 @@
         <f t="shared" si="10"/>
         <v>64.785276073619627</v>
       </c>
-      <c r="J33" s="5">
+      <c r="J33" s="50">
         <f>J27/J30</f>
         <v>64.785276073619627</v>
       </c>
@@ -8950,6 +8960,9 @@
       </c>
     </row>
     <row r="34" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="D34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="J34" s="49"/>
       <c r="AA34" t="s">
         <v>6</v>
       </c>
@@ -8972,8 +8985,8 @@
       <c r="C35" t="s">
         <v>282</v>
       </c>
-      <c r="D35" t="s">
-        <v>314</v>
+      <c r="D35" s="49" t="s">
+        <v>164</v>
       </c>
       <c r="E35" t="s">
         <v>282</v>
@@ -8984,13 +8997,13 @@
       <c r="G35" t="s">
         <v>285</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="49" t="s">
         <v>282</v>
       </c>
       <c r="I35" t="s">
         <v>282</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="49" t="s">
         <v>282</v>
       </c>
       <c r="K35" t="s">
@@ -9019,31 +9032,31 @@
         <v>165</v>
       </c>
       <c r="C36" t="s">
-        <v>316</v>
-      </c>
-      <c r="D36" t="s">
+        <v>314</v>
+      </c>
+      <c r="D36" s="49" t="s">
         <v>163</v>
       </c>
       <c r="E36" t="s">
         <v>165</v>
       </c>
       <c r="F36" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G36" t="s">
         <v>165</v>
       </c>
-      <c r="H36" t="s">
-        <v>316</v>
+      <c r="H36" s="49" t="s">
+        <v>314</v>
       </c>
       <c r="I36" t="s">
-        <v>316</v>
-      </c>
-      <c r="J36" t="s">
-        <v>316</v>
+        <v>314</v>
+      </c>
+      <c r="J36" s="49" t="s">
+        <v>314</v>
       </c>
       <c r="K36" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="R36" t="s">
         <v>102</v>
@@ -9074,7 +9087,7 @@
         <v>0.9</v>
       </c>
       <c r="AA37" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="AB37" s="20">
         <f>(AB29*AB30)/AB36</f>
@@ -9086,9 +9099,6 @@
       </c>
     </row>
     <row r="38" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
-        <v>315</v>
-      </c>
       <c r="M38" s="17" t="s">
         <v>296</v>
       </c>
@@ -9107,7 +9117,7 @@
         <v>2.9320800000000005</v>
       </c>
       <c r="AD38" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="2:30" x14ac:dyDescent="0.2">
@@ -9141,7 +9151,7 @@
         <v>9.6196850393700792</v>
       </c>
       <c r="AD39" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.2">
@@ -9166,7 +9176,7 @@
         <v>278</v>
       </c>
       <c r="AA40" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AB40">
         <v>1.5</v>
@@ -10117,7 +10127,7 @@
     </row>
     <row r="104" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K104" s="7">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="L104" t="s">
         <v>123</v>
@@ -10126,16 +10136,16 @@
     <row r="105" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K105" s="5">
         <f>K104/K92*K95</f>
-        <v>90.022505626406598</v>
+        <v>67.516879219804949</v>
       </c>
       <c r="L105" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="106" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K106" s="2">
         <f>K100/K104</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="L106" t="s">
         <v>125</v>
@@ -10143,7 +10153,7 @@
     </row>
     <row r="108" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K108" s="7">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="L108" t="s">
         <v>305</v>
@@ -10152,7 +10162,7 @@
     <row r="110" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K110">
         <f>K104*K108</f>
-        <v>100000</v>
+        <v>120000</v>
       </c>
       <c r="L110" t="s">
         <v>126</v>
@@ -10161,7 +10171,7 @@
     <row r="111" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K111" s="2">
         <f t="shared" ref="K111" si="15">K100/K110*1000</f>
-        <v>4</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="L111" t="s">
         <v>130</v>
@@ -10195,7 +10205,7 @@
     <row r="116" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K116">
         <f>K113*K106</f>
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="L116" t="s">
         <v>128</v>
@@ -10204,7 +10214,7 @@
     <row r="117" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K117" s="2">
         <f t="shared" ref="K117:L117" si="16">K113*(K111/1000)</f>
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="L117" t="s">
         <v>129</v>
@@ -10231,7 +10241,7 @@
     <row r="122" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K122" s="5">
         <f t="shared" ref="K122:L122" si="19">K116/K119</f>
-        <v>121.47239263803681</v>
+        <v>161.96319018404907</v>
       </c>
       <c r="L122" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
add pids fpr psa and vpsa
</commit_message>
<xml_diff>
--- a/EHD/weight-model.xlsx
+++ b/EHD/weight-model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickos01/Desktop/MolecularKinetics/EHD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5018B18C-0DB4-7941-A13C-CED6740B3C1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2D9098-7E7A-964B-829A-FC0C692F7976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="16860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="336">
   <si>
     <t>Coil form</t>
   </si>
@@ -561,9 +561,6 @@
     <t>45-49g</t>
   </si>
   <si>
-    <t>900mAh</t>
-  </si>
-  <si>
     <t>1600mAh</t>
   </si>
   <si>
@@ -1042,6 +1039,9 @@
   </si>
   <si>
     <t>load capacitance</t>
+  </si>
+  <si>
+    <t>1200mAh</t>
   </si>
 </sst>
 </file>
@@ -5144,8 +5144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Z121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5167,10 +5167,10 @@
         <v>1.1000000000000001E-11</v>
       </c>
       <c r="G2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -5189,7 +5189,7 @@
         <v>1.5999999999999999E-6</v>
       </c>
       <c r="G3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H3" s="5">
         <f>F4*F3/F2</f>
@@ -5211,7 +5211,7 @@
         <v>1.25E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S4">
         <v>2</v>
@@ -5228,7 +5228,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S5">
         <v>37</v>
@@ -5250,10 +5250,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D6" t="s">
         <v>334</v>
-      </c>
-      <c r="D6" t="s">
-        <v>335</v>
       </c>
       <c r="J6">
         <v>2.54</v>
@@ -5363,7 +5363,7 @@
         <v>163</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="N9" s="9" t="s">
         <v>164</v>
@@ -5408,7 +5408,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="7">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
         <v>111</v>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="C12" s="2">
         <f>(C10/1000)*C9* C11</f>
-        <v>13.387500000000003</v>
+        <v>10.237500000000001</v>
       </c>
       <c r="D12" t="s">
         <v>95</v>
@@ -5739,10 +5739,10 @@
     </row>
     <row r="16" spans="1:26">
       <c r="B16">
-        <v>121.5</v>
+        <v>105</v>
       </c>
       <c r="C16">
-        <v>121.5</v>
+        <v>140.22</v>
       </c>
       <c r="D16" t="s">
         <v>85</v>
@@ -5806,11 +5806,11 @@
     <row r="17" spans="2:22">
       <c r="B17" s="5">
         <f>(B14/12000)*B16</f>
-        <v>46.042985581471157</v>
+        <v>39.790234453123219</v>
       </c>
       <c r="C17" s="5">
         <f>(C14/12000)*C16</f>
-        <v>46.042985581471157</v>
+        <v>53.137015952542264</v>
       </c>
       <c r="D17" t="s">
         <v>86</v>
@@ -5856,7 +5856,7 @@
         <v>121.5</v>
       </c>
       <c r="M18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N18" s="2">
         <f>PI()*(N12/2)^2</f>
@@ -5897,7 +5897,7 @@
       </c>
       <c r="C19" s="2">
         <f>(0.29*C12+(0.41*(C13/2))+(1.94*SQRT(((C13/2)^3)/C12)))</f>
-        <v>4.7806486944273656</v>
+        <v>3.9392971842606475</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="C22" s="15">
         <f>((((C9^2) * ((C13/2)^2)) /(( 9 * (C13/2)) + ( 10 * C12))))</f>
-        <v>3674.3410669191912</v>
+        <v>4716.4961507293356</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -6066,7 +6066,7 @@
       </c>
       <c r="C25" s="16">
         <f>1/(2*PI() * SQRT( (C22*0.000001) * ((C20+$B6)*0.000000000001) ) )</f>
-        <v>639013.77227889106</v>
+        <v>564014.42254131637</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="C26" s="2">
         <f>2000000*PI() * SQRT( (C22*0.000001) * ((C20+$B4)*0.000000000001) )</f>
-        <v>1.5649114985953076</v>
+        <v>1.7730043063335779</v>
       </c>
       <c r="D26" t="s">
         <v>69</v>
@@ -6118,7 +6118,7 @@
       </c>
       <c r="C27" s="5">
         <f xml:space="preserve"> 2*PI()*C25</f>
-        <v>4015041.9450681303</v>
+        <v>3543807.1327489777</v>
       </c>
       <c r="D27" t="s">
         <v>81</v>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="C29" s="16">
         <f>C27*(C22/1000000)</f>
-        <v>14752.633504166939</v>
+        <v>16714.352700537718</v>
       </c>
       <c r="D29" t="s">
         <v>82</v>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="C30" s="16">
         <f>1/(C27*((C20+$B6)/1000000000000))</f>
-        <v>14752.633504166934</v>
+        <v>16714.352700537711</v>
       </c>
       <c r="D30" t="s">
         <v>83</v>
@@ -6160,11 +6160,11 @@
     <row r="32" spans="2:22">
       <c r="B32" s="14">
         <f>B29/B17</f>
-        <v>320.4100107292731</v>
+        <v>370.76015527244459</v>
       </c>
       <c r="C32" s="14">
         <f>C29/C17</f>
-        <v>320.4100107292731</v>
+        <v>314.55196346489691</v>
       </c>
       <c r="D32" t="s">
         <v>87</v>
@@ -6173,128 +6173,109 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:11">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:11">
       <c r="A34" s="18" t="s">
         <v>94</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="L34" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="C34" s="29"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:11">
       <c r="B35">
         <v>0.34799999999999998</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35">
+        <v>0.252</v>
+      </c>
+      <c r="D35" t="s">
         <v>89</v>
       </c>
-      <c r="E35">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="F35">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="G35">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="H35">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="I35">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="J35">
-        <v>0.252</v>
-      </c>
-      <c r="K35">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="L35">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="G35" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="B36" s="13">
         <f>1000/B35</f>
         <v>2873.5632183908046</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="13">
+        <f>1000/C35</f>
+        <v>3968.2539682539682</v>
+      </c>
+      <c r="D36" t="s">
         <v>5</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>8</v>
       </c>
-      <c r="E36">
-        <v>0.185</v>
-      </c>
-      <c r="F36">
-        <v>0.247</v>
-      </c>
       <c r="G36">
-        <v>0.308</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="H36">
-        <v>0.37</v>
+        <v>0.252</v>
       </c>
       <c r="I36">
-        <v>0.154</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="J36">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="L36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="B37">
         <f>B10/1000</f>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37">
+        <f>C10/1000</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D37" t="s">
         <v>3</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="G37">
+        <v>0.154</v>
+      </c>
+      <c r="H37">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="J37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="B39" s="1">
         <f>454/(B36*(2.54*0.12))</f>
         <v>0.51834645669291335</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1">
+        <f>454/(C36*(2.54*0.12))</f>
+        <v>0.37535433070866137</v>
+      </c>
+      <c r="D39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:11">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -6302,7 +6283,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:11">
       <c r="B42">
         <v>1.27</v>
       </c>
@@ -6313,7 +6294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:11">
       <c r="B44">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -6324,7 +6305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:11">
       <c r="B45">
         <f>B44*25.4</f>
         <v>0.43180000000000002</v>
@@ -6333,7 +6314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:11">
       <c r="B46">
         <f>B13*25.4</f>
         <v>49.021999999999998</v>
@@ -6353,7 +6334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:11">
       <c r="B47">
         <f>B13</f>
         <v>1.93</v>
@@ -6369,7 +6350,7 @@
         <v>0.66060214111159432</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:11">
       <c r="B48">
         <v>350</v>
       </c>
@@ -6391,7 +6372,7 @@
         <v>10.591358206600455</v>
       </c>
       <c r="K48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="2:11">
@@ -6474,13 +6455,13 @@
     </row>
     <row r="54" spans="2:11">
       <c r="G54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I54" t="s">
-        <v>175</v>
+        <v>335</v>
       </c>
       <c r="J54">
         <v>600</v>
@@ -6525,7 +6506,7 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G59" s="2">
         <f>B59</f>
@@ -6566,7 +6547,7 @@
     </row>
     <row r="64" spans="2:11">
       <c r="I64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -6623,7 +6604,7 @@
         <v>7</v>
       </c>
       <c r="I68" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J68">
         <v>1.2</v>
@@ -6644,7 +6625,7 @@
         <v>130</v>
       </c>
       <c r="D69" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E69">
         <v>4</v>
@@ -6653,7 +6634,7 @@
         <v>0.7</v>
       </c>
       <c r="I69" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J69">
         <v>0.75</v>
@@ -6675,7 +6656,7 @@
         <v>18</v>
       </c>
       <c r="I70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J70">
         <v>1</v>
@@ -6767,7 +6748,7 @@
         <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="2:9">
@@ -6779,12 +6760,12 @@
         <v>48</v>
       </c>
       <c r="G82" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="2:9">
       <c r="G83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H83" s="29">
         <v>25</v>
@@ -6805,7 +6786,7 @@
         <v>31</v>
       </c>
       <c r="G84" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H84" s="29">
         <v>100</v>
@@ -6816,7 +6797,7 @@
     </row>
     <row r="85" spans="2:9">
       <c r="G85" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H85" s="29">
         <v>1.6</v>
@@ -6834,7 +6815,7 @@
         <v>27</v>
       </c>
       <c r="G86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H86" s="29">
         <v>60</v>
@@ -6845,13 +6826,13 @@
     </row>
     <row r="87" spans="2:9">
       <c r="G87" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H87" s="29">
         <v>0.8</v>
       </c>
       <c r="I87" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="2:9">
@@ -6866,13 +6847,13 @@
         <v>28</v>
       </c>
       <c r="G88" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H88" s="29">
         <v>75</v>
       </c>
       <c r="I88" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="2:9">
@@ -6921,7 +6902,7 @@
         <v>0.22771805121324112</v>
       </c>
       <c r="G95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="2:9">
@@ -7006,7 +6987,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="C105" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -7090,7 +7071,7 @@
         <v>45</v>
       </c>
       <c r="D118" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="2:4">
@@ -7108,7 +7089,7 @@
         <v>13.360715576296519</v>
       </c>
       <c r="C121" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -7132,7 +7113,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -7145,7 +7126,7 @@
         <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -7530,7 +7511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AJ129"/>
   <sheetViews>
-    <sheetView topLeftCell="K17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
@@ -7548,25 +7529,25 @@
   <sheetData>
     <row r="2" spans="1:36">
       <c r="A2" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" t="s">
         <v>329</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>330</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>331</v>
-      </c>
-      <c r="F2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:36">
       <c r="B3" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C3">
         <v>9.9</v>
@@ -7585,7 +7566,7 @@
     </row>
     <row r="4" spans="1:36">
       <c r="B4" s="29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C4">
         <v>13.2</v>
@@ -7772,10 +7753,10 @@
         <v>119</v>
       </c>
       <c r="O10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AH10" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:36">
@@ -7929,10 +7910,10 @@
         <v>98</v>
       </c>
       <c r="N13" s="49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T13" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AH13">
         <v>50</v>
@@ -7953,43 +7934,43 @@
       <c r="M14" s="44"/>
       <c r="N14" s="49"/>
       <c r="P14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T14" s="34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U14" s="35" t="s">
         <v>130</v>
       </c>
       <c r="V14" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="W14" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="W14" s="35" t="s">
-        <v>254</v>
-      </c>
       <c r="X14" s="35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y14" s="35" t="s">
         <v>159</v>
       </c>
       <c r="Z14" s="35" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA14" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB14" s="35" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC14" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="AD14" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="AA14" s="35" t="s">
-        <v>257</v>
-      </c>
-      <c r="AB14" s="35" t="s">
-        <v>324</v>
-      </c>
-      <c r="AC14" s="35" t="s">
-        <v>323</v>
-      </c>
-      <c r="AD14" s="35" t="s">
-        <v>259</v>
-      </c>
       <c r="AE14" s="35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF14" s="36"/>
       <c r="AH14">
@@ -8038,7 +8019,7 @@
       </c>
       <c r="N15" s="49"/>
       <c r="P15" s="34" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q15" s="35"/>
       <c r="R15" s="36"/>
@@ -8143,7 +8124,7 @@
       </c>
       <c r="N16" s="49"/>
       <c r="P16" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q16" s="32">
         <v>3.5000000000000003E-2</v>
@@ -8258,7 +8239,7 @@
       </c>
       <c r="N17" s="49"/>
       <c r="P17" s="39" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q17" s="33">
         <f>C16/2</f>
@@ -8340,7 +8321,7 @@
       <c r="M18" s="44"/>
       <c r="N18" s="49"/>
       <c r="P18" s="39" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q18" s="33">
         <f>Q17*Q16</f>
@@ -8529,11 +8510,11 @@
         <v>90.225563909774436</v>
       </c>
       <c r="M20" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N20" s="49"/>
       <c r="P20" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q20" s="33">
         <f>2*Q19</f>
@@ -8743,7 +8724,7 @@
         <v>300</v>
       </c>
       <c r="M23" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N23" s="49"/>
     </row>
@@ -8762,7 +8743,7 @@
       <c r="M24" s="44"/>
       <c r="N24" s="49"/>
       <c r="P24" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="2:36">
@@ -8821,7 +8802,7 @@
         <v>625000</v>
       </c>
       <c r="Q25" s="35" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R25" s="36"/>
     </row>
@@ -8874,18 +8855,18 @@
         <v>129</v>
       </c>
       <c r="N26" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P26" s="39">
         <v>15</v>
       </c>
       <c r="Q26" s="44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="R26" s="49"/>
       <c r="S26" s="31"/>
       <c r="T26" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="2:36">
@@ -8922,7 +8903,7 @@
       <c r="X27" s="36"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="46" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AB27" s="35"/>
       <c r="AC27" s="47">
@@ -8931,7 +8912,7 @@
       <c r="AD27" s="36"/>
       <c r="AF27" s="34"/>
       <c r="AG27" s="46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AH27" s="35"/>
       <c r="AI27" s="47">
@@ -8974,7 +8955,7 @@
         <v>300</v>
       </c>
       <c r="M28" s="44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N28" s="49"/>
       <c r="P28" s="75">
@@ -8982,7 +8963,7 @@
         <v>3926990.8169872416</v>
       </c>
       <c r="Q28" s="44" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="R28" s="49"/>
       <c r="S28" s="31"/>
@@ -9002,7 +8983,7 @@
         <v>6</v>
       </c>
       <c r="AB28" s="44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AC28" s="33"/>
       <c r="AD28" s="49"/>
@@ -9011,7 +8992,7 @@
         <v>6</v>
       </c>
       <c r="AH28" s="44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AI28" s="33"/>
       <c r="AJ28" s="49"/>
@@ -9051,7 +9032,7 @@
         <v>300</v>
       </c>
       <c r="M29" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N29" s="49"/>
       <c r="P29" s="75">
@@ -9078,7 +9059,7 @@
         <v>24</v>
       </c>
       <c r="AB29" s="44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AC29" s="33">
         <f>(AA29*AA30)/(AA28/2)</f>
@@ -9090,7 +9071,7 @@
         <v>16</v>
       </c>
       <c r="AH29" s="44" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AI29" s="33">
         <f>(AG29*AG30)/(AG28/2)</f>
@@ -9152,12 +9133,12 @@
         <v>1.767145867644259E-2</v>
       </c>
       <c r="Q30" s="44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R30" s="49"/>
       <c r="S30" s="31"/>
       <c r="T30" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U30" s="44">
         <v>1</v>
@@ -9166,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="W30" s="44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X30" s="49"/>
       <c r="Z30" s="39"/>
@@ -9174,7 +9155,7 @@
         <v>4</v>
       </c>
       <c r="AB30" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AC30" s="33"/>
       <c r="AD30" s="49"/>
@@ -9183,7 +9164,7 @@
         <v>5</v>
       </c>
       <c r="AH30" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AI30" s="33"/>
       <c r="AJ30" s="49"/>
@@ -9242,7 +9223,7 @@
         <v>5.3014376029327774</v>
       </c>
       <c r="Q31" s="42" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R31" s="43"/>
       <c r="T31" s="39"/>
@@ -9255,7 +9236,7 @@
         <v>1</v>
       </c>
       <c r="AB31" s="44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AC31" s="33"/>
       <c r="AD31" s="49"/>
@@ -9264,7 +9245,7 @@
         <v>1</v>
       </c>
       <c r="AH31" s="44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AI31" s="33"/>
       <c r="AJ31" s="49"/>
@@ -9320,7 +9301,7 @@
       <c r="N32" s="49"/>
       <c r="S32" s="31"/>
       <c r="T32" s="39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U32" s="44">
         <v>3.2000000000000001E-2</v>
@@ -9334,10 +9315,10 @@
       <c r="X32" s="49"/>
       <c r="Z32" s="39"/>
       <c r="AA32" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB32" s="44" t="s">
         <v>284</v>
-      </c>
-      <c r="AB32" s="44" t="s">
-        <v>285</v>
       </c>
       <c r="AC32" s="33">
         <f>AC27*AC29</f>
@@ -9346,10 +9327,10 @@
       <c r="AD32" s="49"/>
       <c r="AF32" s="39"/>
       <c r="AG32" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH32" s="44" t="s">
         <v>284</v>
-      </c>
-      <c r="AH32" s="44" t="s">
-        <v>285</v>
       </c>
       <c r="AI32" s="33">
         <f>AI27*AI29</f>
@@ -9457,7 +9438,7 @@
         <v>2.4696969696969697</v>
       </c>
       <c r="M34" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N34" s="49"/>
       <c r="S34" s="31"/>
@@ -9516,7 +9497,7 @@
       <c r="M35" s="44"/>
       <c r="N35" s="49"/>
       <c r="T35" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="U35" s="44">
         <f>(U28-U27)/2*U29/100</f>
@@ -9603,7 +9584,7 @@
       </c>
       <c r="N36" s="49"/>
       <c r="T36" s="39" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U36" s="66">
         <f>PI() * (U28-((U28-U27)/2)) /10 * U35</f>
@@ -9695,7 +9676,7 @@
         <v>132</v>
       </c>
       <c r="N37" s="49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T37" s="39" t="s">
         <v>8</v>
@@ -9781,42 +9762,42 @@
     </row>
     <row r="39" spans="2:36">
       <c r="B39" s="39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D39" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E39" s="74" t="s">
         <v>162</v>
       </c>
       <c r="F39" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G39" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H39" s="44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I39" s="74" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J39" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K39" s="74" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L39" s="44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M39" s="44"/>
       <c r="N39" s="49"/>
       <c r="T39" s="39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U39" s="33">
         <f>((U28-U27) + (2*U29)  + (2*U33))/10* U30</f>
@@ -9836,7 +9817,7 @@
         <v>11.5824</v>
       </c>
       <c r="AB39" s="44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AC39" s="33"/>
       <c r="AD39" s="49"/>
@@ -9846,7 +9827,7 @@
         <v>7.3152000000000008</v>
       </c>
       <c r="AH39" s="44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AI39" s="33"/>
       <c r="AJ39" s="49"/>
@@ -9859,7 +9840,7 @@
         <v>163</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E40" s="83" t="s">
         <v>161</v>
@@ -9868,27 +9849,27 @@
         <v>163</v>
       </c>
       <c r="G40" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H40" s="42" t="s">
         <v>163</v>
       </c>
       <c r="I40" s="83" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J40" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K40" s="83" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L40" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M40" s="42"/>
       <c r="N40" s="43"/>
       <c r="T40" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U40" s="56">
         <f xml:space="preserve"> PI() * (U27-U33)</f>
@@ -9908,7 +9889,7 @@
         <v>3.5051999999999999</v>
       </c>
       <c r="AB40" s="44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AC40" s="33"/>
       <c r="AD40" s="49"/>
@@ -9918,14 +9899,14 @@
         <v>3.3782000000000005</v>
       </c>
       <c r="AH40" s="44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AI40" s="33"/>
       <c r="AJ40" s="49"/>
     </row>
     <row r="41" spans="2:36">
       <c r="T41" s="39" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U41" s="67">
         <f>(U33*U34)/U40</f>
@@ -9950,7 +9931,7 @@
     </row>
     <row r="42" spans="2:36">
       <c r="T42" s="39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U42" s="33">
         <f>U34*U39 /100</f>
@@ -9961,7 +9942,7 @@
         <v>2.9320800000000005</v>
       </c>
       <c r="W42" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="X42" s="49"/>
       <c r="Z42" s="39"/>
@@ -9977,7 +9958,7 @@
     </row>
     <row r="43" spans="2:36">
       <c r="T43" s="39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U43" s="56">
         <f>U42*100 / (2.54 * 12)</f>
@@ -9988,7 +9969,7 @@
         <v>9.6196850393700792</v>
       </c>
       <c r="W43" s="44" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="X43" s="49"/>
       <c r="Z43" s="39"/>
@@ -10003,14 +9984,14 @@
         <v>0.70699999999999996</v>
       </c>
       <c r="AH43" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AI43" s="44"/>
       <c r="AJ43" s="49"/>
     </row>
     <row r="44" spans="2:36">
       <c r="T44" s="39" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U44" s="44">
         <v>1.5</v>
@@ -10034,7 +10015,7 @@
         <v>0.42699999999999999</v>
       </c>
       <c r="AH44" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AI44" s="44"/>
       <c r="AJ44" s="49"/>
@@ -10067,14 +10048,14 @@
         <v>0.27999999999999997</v>
       </c>
       <c r="AH45" s="44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AI45" s="44"/>
       <c r="AJ45" s="49"/>
     </row>
     <row r="46" spans="2:36" ht="17" thickBot="1">
       <c r="T46" s="39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U46" s="56">
         <f>U43*3</f>
@@ -10085,7 +10066,7 @@
         <v>28.859055118110238</v>
       </c>
       <c r="W46" s="44" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X46" s="49"/>
       <c r="Z46" s="41"/>
@@ -10102,7 +10083,7 @@
         <v>0.13999999999999999</v>
       </c>
       <c r="AH46" s="42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AI46" s="42"/>
       <c r="AJ46" s="43"/>
@@ -10125,19 +10106,19 @@
         <v>1.6177374218750664</v>
       </c>
       <c r="W48" s="42" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X48" s="43"/>
     </row>
     <row r="53" spans="16:33">
       <c r="T53" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="X53" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC53" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="54" spans="16:33">
@@ -10145,22 +10126,22 @@
       <c r="U54" s="32"/>
       <c r="V54" s="52"/>
       <c r="X54" s="51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Y54" s="32">
         <v>2500</v>
       </c>
       <c r="Z54" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AC54" s="51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD54" s="32">
         <v>5000</v>
       </c>
       <c r="AE54" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF54" s="32"/>
       <c r="AG54" s="52"/>
@@ -10174,53 +10155,53 @@
       </c>
       <c r="V55" s="55"/>
       <c r="X55" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y55" s="54">
         <v>4.7000000000000003E-10</v>
       </c>
       <c r="Z55" s="55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC55" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD55" s="54">
         <v>3.9E-10</v>
       </c>
       <c r="AE55" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AF55" s="44"/>
       <c r="AG55" s="55"/>
     </row>
     <row r="56" spans="16:33">
       <c r="T56" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U56" s="44">
         <v>0.9</v>
       </c>
       <c r="V56" s="55"/>
       <c r="X56" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Y56" s="33">
         <f>1-(300/Y54)</f>
         <v>0.88</v>
       </c>
       <c r="Z56" s="55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AC56" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AD56" s="33">
         <f>1-(300/AD54)</f>
         <v>0.94</v>
       </c>
       <c r="AE56" s="44" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AF56" s="44"/>
       <c r="AG56" s="55"/>
@@ -10254,19 +10235,19 @@
         <v>77.792553191489432</v>
       </c>
       <c r="AG57" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="16:33">
       <c r="T58" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U58" s="56">
         <f>3/(0.01*(1-U56))</f>
         <v>3000.0000000000005</v>
       </c>
       <c r="V58" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X58" s="53"/>
       <c r="Y58" s="44"/>
@@ -10277,21 +10258,21 @@
         <v>1296.5425531914896</v>
       </c>
       <c r="AE58" s="44" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF58" s="44"/>
       <c r="AG58" s="55"/>
     </row>
     <row r="59" spans="16:33">
       <c r="T59" s="57" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U59" s="58">
         <f>(1.6*U56)/(U58*U55)</f>
         <v>3.8400000000000002E-10</v>
       </c>
       <c r="V59" s="59" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="X59" s="53"/>
       <c r="Y59" s="44"/>
@@ -10307,22 +10288,22 @@
       <c r="U60" s="32"/>
       <c r="V60" s="52"/>
       <c r="X60" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Y60" s="44">
         <v>2700</v>
       </c>
       <c r="Z60" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AC60" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD60" s="44">
         <v>3500</v>
       </c>
       <c r="AE60" s="44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF60" s="44"/>
       <c r="AG60" s="55"/>
@@ -10336,22 +10317,22 @@
       </c>
       <c r="V61" s="55"/>
       <c r="X61" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y61" s="54">
         <v>4.7000000000000003E-10</v>
       </c>
       <c r="Z61" s="55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC61" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD61" s="54">
         <v>3.9E-10</v>
       </c>
       <c r="AE61" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AF61" s="44"/>
       <c r="AG61" s="55"/>
@@ -10359,31 +10340,31 @@
     <row r="62" spans="16:33">
       <c r="P62" s="2"/>
       <c r="T62" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U62" s="44">
         <v>0.88</v>
       </c>
       <c r="V62" s="55"/>
       <c r="X62" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Y62" s="33">
         <f>1-(300/Y60)</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="Z62" s="55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AC62" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AD62" s="33">
         <f>1-(300/AD60)</f>
         <v>0.91428571428571426</v>
       </c>
       <c r="AE62" s="44" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AF62" s="44"/>
       <c r="AG62" s="55"/>
@@ -10417,19 +10398,19 @@
         <v>79.980468750000043</v>
       </c>
       <c r="AG63" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="16:33">
       <c r="T64" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U64" s="56">
         <f>3/(0.01*(1-U62))</f>
         <v>2500</v>
       </c>
       <c r="V64" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X64" s="53"/>
       <c r="Y64" s="44"/>
@@ -10440,21 +10421,21 @@
         <v>933.10546875000011</v>
       </c>
       <c r="AE64" s="44" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF64" s="44"/>
       <c r="AG64" s="55"/>
     </row>
     <row r="65" spans="20:33">
       <c r="T65" s="57" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U65" s="58">
         <f>(1.6*U62)/(U64*U61)</f>
         <v>4.6933333333333337E-10</v>
       </c>
       <c r="V65" s="59" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="X65" s="53"/>
       <c r="Y65" s="44"/>
@@ -10467,68 +10448,68 @@
     </row>
     <row r="66" spans="20:33">
       <c r="X66" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Y66" s="44">
         <v>3000</v>
       </c>
       <c r="Z66" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AC66" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD66" s="44">
         <v>3000</v>
       </c>
       <c r="AE66" s="44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF66" s="44"/>
       <c r="AG66" s="55"/>
     </row>
     <row r="67" spans="20:33">
       <c r="X67" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y67" s="54">
         <v>4.7000000000000003E-10</v>
       </c>
       <c r="Z67" s="55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC67" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD67" s="54">
         <v>3.9E-10</v>
       </c>
       <c r="AE67" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AF67" s="44"/>
       <c r="AG67" s="55"/>
     </row>
     <row r="68" spans="20:33">
       <c r="X68" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Y68" s="33">
         <f>1-(300/Y66)</f>
         <v>0.9</v>
       </c>
       <c r="Z68" s="55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AC68" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AD68" s="33">
         <f>1-(300/AD66)</f>
         <v>0.9</v>
       </c>
       <c r="AE68" s="44" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AF68" s="44"/>
       <c r="AG68" s="55"/>
@@ -10559,7 +10540,7 @@
         <v>81.249999999999957</v>
       </c>
       <c r="AG69" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="70" spans="20:33">
@@ -10572,7 +10553,7 @@
         <v>812.49999999999989</v>
       </c>
       <c r="AE70" s="44" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF70" s="44"/>
       <c r="AG70" s="55"/>
@@ -10589,75 +10570,75 @@
     </row>
     <row r="72" spans="20:33">
       <c r="X72" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Y72" s="44">
         <v>2200</v>
       </c>
       <c r="Z72" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AC72" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AD72" s="44">
         <v>2500</v>
       </c>
       <c r="AE72" s="44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF72" s="44"/>
       <c r="AG72" s="55"/>
     </row>
     <row r="73" spans="20:33">
       <c r="X73" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Y73" s="54">
         <v>4.7000000000000003E-10</v>
       </c>
       <c r="Z73" s="55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC73" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AD73" s="54">
         <v>3.9E-10</v>
       </c>
       <c r="AE73" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AF73" s="44"/>
       <c r="AG73" s="55"/>
     </row>
     <row r="74" spans="20:33">
       <c r="X74" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Y74" s="33">
         <f>1-(300/Y72)</f>
         <v>0.86363636363636365</v>
       </c>
       <c r="Z74" s="55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AA74" s="5">
         <f>1/Y75*(1-Y74)*1000000000</f>
         <v>102.03947368421052</v>
       </c>
       <c r="AB74" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AC74" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AD74" s="33">
         <f>1-(300/AD72)</f>
         <v>0.88</v>
       </c>
       <c r="AE74" s="44" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AF74" s="44"/>
       <c r="AG74" s="55"/>
@@ -10692,7 +10673,7 @@
         <v>83.096590909090892</v>
       </c>
       <c r="AG75" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="76" spans="20:33">
@@ -10702,7 +10683,7 @@
         <v>692.47159090909076</v>
       </c>
       <c r="AE76" s="62" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF76" s="62"/>
       <c r="AG76" s="59"/>
@@ -10814,7 +10795,7 @@
         <v>67.516879219804949</v>
       </c>
       <c r="M109" s="49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="110" spans="12:13">
@@ -10835,7 +10816,7 @@
         <v>400</v>
       </c>
       <c r="M112" s="49" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="113" spans="12:13">
@@ -10869,7 +10850,7 @@
         <v>300</v>
       </c>
       <c r="M117" s="49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="118" spans="12:13">
@@ -10877,7 +10858,7 @@
         <v>300</v>
       </c>
       <c r="M118" s="49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="119" spans="12:13">
@@ -10917,7 +10898,7 @@
         <v>2.4696969696969697</v>
       </c>
       <c r="M123" s="49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="124" spans="12:13">
@@ -10990,29 +10971,29 @@
     </row>
     <row r="5" spans="3:11">
       <c r="H5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="3:11">
       <c r="C6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="3:11" ht="19">
       <c r="C7" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="24">
         <v>30</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H7">
         <v>30</v>
@@ -11023,7 +11004,7 @@
     </row>
     <row r="8" spans="3:11" ht="19">
       <c r="C8" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D8" s="24">
         <v>0.30099999999999999</v>
@@ -11040,7 +11021,7 @@
     </row>
     <row r="9" spans="3:11" ht="19">
       <c r="C9" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D9" s="26">
         <v>21</v>
@@ -11058,7 +11039,7 @@
     </row>
     <row r="10" spans="3:11" ht="19">
       <c r="C10" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D10" s="26">
         <v>2.5000000000000001E-2</v>
@@ -11077,7 +11058,7 @@
         <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="3:11" ht="19">
@@ -11089,25 +11070,25 @@
         <v>87.110734542640927</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="3:11" ht="19">
       <c r="C12" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12" s="28">
         <f>D11*D10*LOG(D9/D10,2.718)</f>
         <v>14.665310181214844</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H12">
         <v>0.1</v>
@@ -11120,12 +11101,12 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="3:11">
       <c r="C14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H14" t="s">
         <v>120</v>
@@ -11133,13 +11114,13 @@
     </row>
     <row r="15" spans="3:11" ht="19">
       <c r="C15" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" s="24">
         <v>30</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H15">
         <f>H12*H9</f>
@@ -11153,12 +11134,12 @@
         <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="3:11" ht="19">
       <c r="C16" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="24">
         <v>0.30099999999999999</v>
@@ -11169,7 +11150,7 @@
     </row>
     <row r="17" spans="3:10" ht="19">
       <c r="C17" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="26">
         <v>21</v>
@@ -11180,7 +11161,7 @@
     </row>
     <row r="18" spans="3:10" ht="19">
       <c r="C18" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="26">
         <v>0.6</v>
@@ -11198,71 +11179,71 @@
         <v>41.657679872084323</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="19">
       <c r="C20" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="28">
         <f>D19*D18*LOG(D17/D18,2.718)</f>
         <v>88.87374563714863</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I20" s="4">
         <f>D12*2</f>
         <v>29.330620362429688</v>
       </c>
       <c r="J20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="3:10">
       <c r="H21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I21" s="4">
         <f>D28</f>
         <v>205.59078000666895</v>
       </c>
       <c r="J21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="3:10">
       <c r="C22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I22">
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="3:10" ht="19">
       <c r="C23" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D23" s="24">
         <v>30</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="3:10" ht="19">
       <c r="C24" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D24" s="24">
         <v>0.30099999999999999</v>
@@ -11273,7 +11254,7 @@
     </row>
     <row r="25" spans="3:10" ht="19">
       <c r="C25" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D25" s="26">
         <v>25</v>
@@ -11282,7 +11263,7 @@
         <v>130</v>
       </c>
       <c r="H25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I25" t="s">
         <v>143</v>
@@ -11290,7 +11271,7 @@
     </row>
     <row r="26" spans="3:10" ht="19">
       <c r="C26" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D26" s="26">
         <v>2.5</v>
@@ -11299,7 +11280,7 @@
         <v>130</v>
       </c>
       <c r="H26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I26">
         <v>0.127</v>
@@ -11314,10 +11295,10 @@
         <v>35.711073454264096</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I27">
         <v>0.25459999999999999</v>
@@ -11325,17 +11306,17 @@
     </row>
     <row r="28" spans="3:10" ht="19">
       <c r="C28" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D28" s="28">
         <f>D27*D26*LOG(D25/D26,2.718)</f>
         <v>205.59078000666895</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I28">
         <v>0.3211</v>
@@ -11351,7 +11332,7 @@
     </row>
     <row r="30" spans="3:10">
       <c r="C30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H30" t="s">
         <v>167</v>
@@ -11362,16 +11343,16 @@
     </row>
     <row r="31" spans="3:10" ht="19">
       <c r="C31" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D31" s="24">
         <v>30</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I31">
         <v>0.64380000000000004</v>
@@ -11379,7 +11360,7 @@
     </row>
     <row r="32" spans="3:10" ht="19">
       <c r="C32" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D32" s="24">
         <v>0.30099999999999999</v>
@@ -11390,7 +11371,7 @@
     </row>
     <row r="33" spans="3:22" ht="19">
       <c r="C33" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D33" s="26">
         <v>25</v>
@@ -11399,7 +11380,7 @@
         <v>130</v>
       </c>
       <c r="J33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K33">
         <v>10</v>
@@ -11440,7 +11421,7 @@
     </row>
     <row r="34" spans="3:22" ht="19">
       <c r="C34" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D34" s="26">
         <v>5</v>
@@ -11449,7 +11430,7 @@
         <v>130</v>
       </c>
       <c r="J34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K34">
         <f t="shared" ref="K34:V34" si="0">K39-K40</f>
@@ -11509,10 +11490,10 @@
         <v>34.038338767364621</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K35" s="4">
         <f t="shared" ref="K35:V35" si="1">$D$12</f>
@@ -11565,17 +11546,17 @@
     </row>
     <row r="36" spans="3:22" ht="19">
       <c r="C36" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D36" s="28">
         <f>D35*D34*LOG(D33/D34,2.718)</f>
         <v>273.94136785339589</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K36" s="4">
         <f t="shared" ref="K36:V36" si="2">$D$20</f>
@@ -11628,7 +11609,7 @@
     </row>
     <row r="37" spans="3:22">
       <c r="J37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K37">
         <v>21</v>
@@ -11669,10 +11650,10 @@
     </row>
     <row r="38" spans="3:22">
       <c r="C38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -11713,16 +11694,16 @@
     </row>
     <row r="39" spans="3:22" ht="19">
       <c r="C39" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D39" s="24">
         <v>30</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K39">
         <f t="shared" ref="K39:V39" si="3">MAX(0, (K$38*K$33*(K$33-K35))/K$37)</f>
@@ -11775,7 +11756,7 @@
     </row>
     <row r="40" spans="3:22" ht="19">
       <c r="C40" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D40" s="24">
         <v>0.30099999999999999</v>
@@ -11784,7 +11765,7 @@
         <v>130</v>
       </c>
       <c r="J40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K40">
         <f t="shared" ref="K40:V40" si="4">MAX(0, (K$38*K$33*(K$33-K36))/K$37)</f>
@@ -11837,7 +11818,7 @@
     </row>
     <row r="41" spans="3:22" ht="19">
       <c r="C41" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D41" s="26">
         <v>25</v>
@@ -11848,7 +11829,7 @@
     </row>
     <row r="42" spans="3:22" ht="19">
       <c r="C42" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D42" s="26">
         <v>1</v>
@@ -11857,7 +11838,7 @@
         <v>130</v>
       </c>
       <c r="J42" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="3:22" ht="19">
@@ -11869,13 +11850,13 @@
         <v>39.03</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I43" s="29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K43">
         <v>10</v>
@@ -11916,17 +11897,17 @@
     </row>
     <row r="44" spans="3:22" ht="19">
       <c r="C44" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D44" s="28">
         <f>D43*D42*LOG(D41/D42,2.718)</f>
         <v>125.64575093270162</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K44" s="2">
         <f>K45/K43*K47</f>
@@ -11976,7 +11957,7 @@
         <v>1.4</v>
       </c>
       <c r="J45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K45" s="2">
         <f t="shared" ref="K45:V45" si="6">K46*$I45</f>
@@ -12029,7 +12010,7 @@
     </row>
     <row r="46" spans="3:22">
       <c r="J46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -12070,10 +12051,10 @@
     </row>
     <row r="47" spans="3:22">
       <c r="C47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -12114,13 +12095,13 @@
     </row>
     <row r="48" spans="3:22" ht="19">
       <c r="C48" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D48" s="24">
         <v>30</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K48" s="4">
         <f>K43*10/12</f>
@@ -12173,7 +12154,7 @@
     </row>
     <row r="49" spans="3:5" ht="19">
       <c r="C49" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D49" s="24">
         <v>0.30099999999999999</v>
@@ -12184,7 +12165,7 @@
     </row>
     <row r="50" spans="3:5" ht="19">
       <c r="C50" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D50" s="26">
         <v>3.7</v>
@@ -12195,7 +12176,7 @@
     </row>
     <row r="51" spans="3:5" ht="19">
       <c r="C51" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D51" s="26">
         <v>0.6</v>
@@ -12213,19 +12194,19 @@
         <v>41.657679872084323</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="3:5" ht="19">
       <c r="C53" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D53" s="28">
         <f>D52*D51*LOG(D50/D51,2.718)</f>
         <v>45.473866968206337</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="10:14">
@@ -12240,7 +12221,7 @@
         <v>85.333333333333329</v>
       </c>
       <c r="N67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="10:14">
@@ -12269,22 +12250,22 @@
     </row>
     <row r="75" spans="10:14">
       <c r="J75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="10:14">
       <c r="J76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="10:14">
       <c r="J78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="10:14">
       <c r="J79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -12540,7 +12521,7 @@
     </row>
     <row r="25" spans="2:7">
       <c r="B25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C25" s="5">
         <f>-C19</f>
@@ -12555,7 +12536,7 @@
     </row>
     <row r="26" spans="2:7">
       <c r="B26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C26" s="5">
         <f>C23</f>
@@ -12641,10 +12622,10 @@
   <sheetData>
     <row r="6" spans="3:5">
       <c r="C6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" t="s">
         <v>223</v>
-      </c>
-      <c r="D6" t="s">
-        <v>224</v>
       </c>
       <c r="E6">
         <v>139439</v>
@@ -12652,10 +12633,10 @@
     </row>
     <row r="7" spans="3:5">
       <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" t="s">
         <v>223</v>
-      </c>
-      <c r="D7" t="s">
-        <v>224</v>
       </c>
       <c r="E7">
         <v>139471</v>
@@ -12663,10 +12644,10 @@
     </row>
     <row r="8" spans="3:5">
       <c r="C8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" t="s">
         <v>223</v>
-      </c>
-      <c r="D8" t="s">
-        <v>224</v>
       </c>
       <c r="E8">
         <v>139341</v>
@@ -12674,10 +12655,10 @@
     </row>
     <row r="9" spans="3:5">
       <c r="C9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" t="s">
         <v>223</v>
-      </c>
-      <c r="D9" t="s">
-        <v>224</v>
       </c>
       <c r="E9">
         <v>139430</v>
@@ -12685,10 +12666,10 @@
     </row>
     <row r="10" spans="3:5">
       <c r="C10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" t="s">
         <v>223</v>
-      </c>
-      <c r="D10" t="s">
-        <v>224</v>
       </c>
       <c r="E10">
         <v>139415</v>
@@ -12696,10 +12677,10 @@
     </row>
     <row r="11" spans="3:5">
       <c r="C11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11" t="s">
         <v>223</v>
-      </c>
-      <c r="D11" t="s">
-        <v>224</v>
       </c>
       <c r="E11">
         <v>139436</v>
@@ -12707,10 +12688,10 @@
     </row>
     <row r="12" spans="3:5">
       <c r="C12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" t="s">
         <v>223</v>
-      </c>
-      <c r="D12" t="s">
-        <v>224</v>
       </c>
       <c r="E12">
         <v>139456</v>
@@ -12718,10 +12699,10 @@
     </row>
     <row r="13" spans="3:5">
       <c r="C13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" t="s">
         <v>223</v>
-      </c>
-      <c r="D13" t="s">
-        <v>224</v>
       </c>
       <c r="E13">
         <v>139436</v>
@@ -12729,10 +12710,10 @@
     </row>
     <row r="14" spans="3:5">
       <c r="C14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D14" t="s">
         <v>223</v>
-      </c>
-      <c r="D14" t="s">
-        <v>224</v>
       </c>
       <c r="E14">
         <v>139461</v>
@@ -12740,10 +12721,10 @@
     </row>
     <row r="15" spans="3:5">
       <c r="C15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" t="s">
         <v>223</v>
-      </c>
-      <c r="D15" t="s">
-        <v>224</v>
       </c>
       <c r="E15">
         <v>139455</v>
@@ -12751,10 +12732,10 @@
     </row>
     <row r="16" spans="3:5">
       <c r="C16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" t="s">
         <v>223</v>
-      </c>
-      <c r="D16" t="s">
-        <v>224</v>
       </c>
       <c r="E16">
         <v>139435</v>
@@ -12762,10 +12743,10 @@
     </row>
     <row r="17" spans="3:6">
       <c r="C17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D17" t="s">
         <v>223</v>
-      </c>
-      <c r="D17" t="s">
-        <v>224</v>
       </c>
       <c r="E17">
         <v>139454</v>
@@ -12773,10 +12754,10 @@
     </row>
     <row r="18" spans="3:6">
       <c r="C18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D18" t="s">
         <v>223</v>
-      </c>
-      <c r="D18" t="s">
-        <v>224</v>
       </c>
       <c r="E18">
         <v>139432</v>
@@ -12784,10 +12765,10 @@
     </row>
     <row r="19" spans="3:6">
       <c r="C19" t="s">
+        <v>222</v>
+      </c>
+      <c r="D19" t="s">
         <v>223</v>
-      </c>
-      <c r="D19" t="s">
-        <v>224</v>
       </c>
       <c r="E19">
         <v>139452</v>
@@ -12795,10 +12776,10 @@
     </row>
     <row r="20" spans="3:6">
       <c r="C20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" t="s">
         <v>223</v>
-      </c>
-      <c r="D20" t="s">
-        <v>224</v>
       </c>
       <c r="E20">
         <v>139444</v>
@@ -12806,10 +12787,10 @@
     </row>
     <row r="21" spans="3:6">
       <c r="C21" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" t="s">
         <v>223</v>
-      </c>
-      <c r="D21" t="s">
-        <v>224</v>
       </c>
       <c r="E21">
         <v>139409</v>
@@ -12817,10 +12798,10 @@
     </row>
     <row r="22" spans="3:6">
       <c r="C22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D22" t="s">
         <v>223</v>
-      </c>
-      <c r="D22" t="s">
-        <v>224</v>
       </c>
       <c r="E22">
         <v>139463</v>
@@ -12828,10 +12809,10 @@
     </row>
     <row r="23" spans="3:6">
       <c r="C23" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" t="s">
         <v>223</v>
-      </c>
-      <c r="D23" t="s">
-        <v>224</v>
       </c>
       <c r="E23">
         <v>139417</v>
@@ -12839,10 +12820,10 @@
     </row>
     <row r="24" spans="3:6">
       <c r="C24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" t="s">
         <v>223</v>
-      </c>
-      <c r="D24" t="s">
-        <v>224</v>
       </c>
       <c r="E24">
         <v>139439</v>
@@ -12850,10 +12831,10 @@
     </row>
     <row r="25" spans="3:6">
       <c r="C25" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" t="s">
         <v>223</v>
-      </c>
-      <c r="D25" t="s">
-        <v>224</v>
       </c>
       <c r="E25">
         <v>139369</v>
@@ -12868,10 +12849,10 @@
     </row>
     <row r="28" spans="3:6">
       <c r="C28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" t="s">
         <v>223</v>
-      </c>
-      <c r="D28" t="s">
-        <v>224</v>
       </c>
       <c r="E28">
         <v>502546</v>
@@ -12879,10 +12860,10 @@
     </row>
     <row r="29" spans="3:6">
       <c r="C29" t="s">
+        <v>222</v>
+      </c>
+      <c r="D29" t="s">
         <v>223</v>
-      </c>
-      <c r="D29" t="s">
-        <v>224</v>
       </c>
       <c r="E29">
         <v>502494</v>
@@ -12890,10 +12871,10 @@
     </row>
     <row r="30" spans="3:6">
       <c r="C30" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" t="s">
         <v>223</v>
-      </c>
-      <c r="D30" t="s">
-        <v>224</v>
       </c>
       <c r="E30">
         <v>502548</v>
@@ -12901,10 +12882,10 @@
     </row>
     <row r="31" spans="3:6">
       <c r="C31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D31" t="s">
         <v>223</v>
-      </c>
-      <c r="D31" t="s">
-        <v>224</v>
       </c>
       <c r="E31">
         <v>502442</v>
@@ -12912,10 +12893,10 @@
     </row>
     <row r="32" spans="3:6">
       <c r="C32" t="s">
+        <v>222</v>
+      </c>
+      <c r="D32" t="s">
         <v>223</v>
-      </c>
-      <c r="D32" t="s">
-        <v>224</v>
       </c>
       <c r="E32">
         <v>502516</v>
@@ -12923,10 +12904,10 @@
     </row>
     <row r="33" spans="3:9">
       <c r="C33" t="s">
+        <v>222</v>
+      </c>
+      <c r="D33" t="s">
         <v>223</v>
-      </c>
-      <c r="D33" t="s">
-        <v>224</v>
       </c>
       <c r="E33">
         <v>502508</v>
@@ -12934,10 +12915,10 @@
     </row>
     <row r="34" spans="3:9">
       <c r="C34" t="s">
+        <v>222</v>
+      </c>
+      <c r="D34" t="s">
         <v>223</v>
-      </c>
-      <c r="D34" t="s">
-        <v>224</v>
       </c>
       <c r="E34">
         <v>502500</v>
@@ -12945,10 +12926,10 @@
     </row>
     <row r="35" spans="3:9">
       <c r="C35" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" t="s">
         <v>223</v>
-      </c>
-      <c r="D35" t="s">
-        <v>224</v>
       </c>
       <c r="E35">
         <v>502542</v>
@@ -12956,10 +12937,10 @@
     </row>
     <row r="36" spans="3:9">
       <c r="C36" t="s">
+        <v>222</v>
+      </c>
+      <c r="D36" t="s">
         <v>223</v>
-      </c>
-      <c r="D36" t="s">
-        <v>224</v>
       </c>
       <c r="E36">
         <v>502523</v>
@@ -12967,10 +12948,10 @@
     </row>
     <row r="37" spans="3:9">
       <c r="C37" t="s">
+        <v>222</v>
+      </c>
+      <c r="D37" t="s">
         <v>223</v>
-      </c>
-      <c r="D37" t="s">
-        <v>224</v>
       </c>
       <c r="E37">
         <v>502559</v>
@@ -12978,10 +12959,10 @@
     </row>
     <row r="38" spans="3:9">
       <c r="C38" t="s">
+        <v>222</v>
+      </c>
+      <c r="D38" t="s">
         <v>223</v>
-      </c>
-      <c r="D38" t="s">
-        <v>224</v>
       </c>
       <c r="E38">
         <v>502555</v>
@@ -12989,10 +12970,10 @@
     </row>
     <row r="39" spans="3:9">
       <c r="C39" t="s">
+        <v>222</v>
+      </c>
+      <c r="D39" t="s">
         <v>223</v>
-      </c>
-      <c r="D39" t="s">
-        <v>224</v>
       </c>
       <c r="E39">
         <v>502494</v>
@@ -13000,10 +12981,10 @@
     </row>
     <row r="40" spans="3:9">
       <c r="C40" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" t="s">
         <v>223</v>
-      </c>
-      <c r="D40" t="s">
-        <v>224</v>
       </c>
       <c r="E40">
         <v>502541</v>
@@ -13011,10 +12992,10 @@
     </row>
     <row r="41" spans="3:9">
       <c r="C41" t="s">
+        <v>222</v>
+      </c>
+      <c r="D41" t="s">
         <v>223</v>
-      </c>
-      <c r="D41" t="s">
-        <v>224</v>
       </c>
       <c r="E41">
         <v>502520</v>
@@ -13022,10 +13003,10 @@
     </row>
     <row r="42" spans="3:9">
       <c r="C42" t="s">
+        <v>222</v>
+      </c>
+      <c r="D42" t="s">
         <v>223</v>
-      </c>
-      <c r="D42" t="s">
-        <v>224</v>
       </c>
       <c r="E42">
         <v>502450</v>
@@ -13033,10 +13014,10 @@
     </row>
     <row r="43" spans="3:9">
       <c r="C43" t="s">
+        <v>222</v>
+      </c>
+      <c r="D43" t="s">
         <v>223</v>
-      </c>
-      <c r="D43" t="s">
-        <v>224</v>
       </c>
       <c r="E43">
         <v>502461</v>
@@ -13044,10 +13025,10 @@
     </row>
     <row r="44" spans="3:9">
       <c r="C44" t="s">
+        <v>222</v>
+      </c>
+      <c r="D44" t="s">
         <v>223</v>
-      </c>
-      <c r="D44" t="s">
-        <v>224</v>
       </c>
       <c r="E44">
         <v>502502</v>
@@ -13055,10 +13036,10 @@
     </row>
     <row r="45" spans="3:9">
       <c r="C45" t="s">
+        <v>222</v>
+      </c>
+      <c r="D45" t="s">
         <v>223</v>
-      </c>
-      <c r="D45" t="s">
-        <v>224</v>
       </c>
       <c r="E45">
         <v>502492</v>
@@ -13066,10 +13047,10 @@
     </row>
     <row r="46" spans="3:9">
       <c r="C46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D46" t="s">
         <v>223</v>
-      </c>
-      <c r="D46" t="s">
-        <v>224</v>
       </c>
       <c r="E46">
         <v>502460</v>
@@ -13077,10 +13058,10 @@
     </row>
     <row r="47" spans="3:9">
       <c r="C47" t="s">
+        <v>222</v>
+      </c>
+      <c r="D47" t="s">
         <v>223</v>
-      </c>
-      <c r="D47" t="s">
-        <v>224</v>
       </c>
       <c r="E47">
         <v>502500</v>
@@ -13088,10 +13069,10 @@
     </row>
     <row r="48" spans="3:9">
       <c r="C48" t="s">
+        <v>222</v>
+      </c>
+      <c r="D48" t="s">
         <v>223</v>
-      </c>
-      <c r="D48" t="s">
-        <v>224</v>
       </c>
       <c r="E48">
         <v>502515</v>
@@ -13101,15 +13082,15 @@
         <v>139432.70000000001</v>
       </c>
       <c r="I48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="3:9">
       <c r="C49" t="s">
+        <v>222</v>
+      </c>
+      <c r="D49" t="s">
         <v>223</v>
-      </c>
-      <c r="D49" t="s">
-        <v>224</v>
       </c>
       <c r="E49">
         <v>502523</v>
@@ -13126,7 +13107,7 @@
         <v>191.79925082841086</v>
       </c>
       <c r="I49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="3:9">

</xml_diff>